<commit_message>
Bugfix for "New" menuitem
</commit_message>
<xml_diff>
--- a/output/flip.xlsx
+++ b/output/flip.xlsx
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191:S194"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221:S224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5725,120 +5725,120 @@
       <c r="S220" s="2"/>
     </row>
     <row r="221" spans="1:19">
-      <c r="A221" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E221" s="2"/>
-      <c r="F221" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J221" s="2"/>
-      <c r="K221" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O221" s="2"/>
-      <c r="P221" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="R221" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S221" s="4" t="s">
+      <c r="A221" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E221" s="11"/>
+      <c r="F221" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J221" s="11"/>
+      <c r="K221" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O221" s="11"/>
+      <c r="P221" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R221" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S221" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:19">
-      <c r="A222" s="5"/>
-      <c r="B222" s="6"/>
-      <c r="C222" s="6"/>
-      <c r="D222" s="6"/>
-      <c r="E222" s="2"/>
-      <c r="F222" s="5"/>
-      <c r="G222" s="6"/>
-      <c r="H222" s="6"/>
-      <c r="I222" s="6"/>
-      <c r="J222" s="2"/>
-      <c r="K222" s="5"/>
-      <c r="L222" s="6"/>
-      <c r="M222" s="6"/>
-      <c r="N222" s="6"/>
-      <c r="O222" s="2"/>
-      <c r="P222" s="5"/>
-      <c r="Q222" s="6"/>
-      <c r="R222" s="6"/>
-      <c r="S222" s="6"/>
+      <c r="A222" s="12"/>
+      <c r="B222" s="13"/>
+      <c r="C222" s="13"/>
+      <c r="D222" s="13"/>
+      <c r="E222" s="11"/>
+      <c r="F222" s="12"/>
+      <c r="G222" s="13"/>
+      <c r="H222" s="13"/>
+      <c r="I222" s="13"/>
+      <c r="J222" s="11"/>
+      <c r="K222" s="12"/>
+      <c r="L222" s="13"/>
+      <c r="M222" s="13"/>
+      <c r="N222" s="13"/>
+      <c r="O222" s="11"/>
+      <c r="P222" s="12"/>
+      <c r="Q222" s="13"/>
+      <c r="R222" s="13"/>
+      <c r="S222" s="13"/>
     </row>
     <row r="223" spans="1:19">
-      <c r="A223" s="5"/>
-      <c r="B223" s="6"/>
-      <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
-      <c r="E223" s="2"/>
-      <c r="F223" s="5"/>
-      <c r="G223" s="6"/>
-      <c r="H223" s="6"/>
-      <c r="I223" s="6"/>
-      <c r="J223" s="2"/>
-      <c r="K223" s="5"/>
-      <c r="L223" s="6"/>
-      <c r="M223" s="6"/>
-      <c r="N223" s="6"/>
-      <c r="O223" s="2"/>
-      <c r="P223" s="5"/>
-      <c r="Q223" s="6"/>
-      <c r="R223" s="6"/>
-      <c r="S223" s="6"/>
+      <c r="A223" s="12"/>
+      <c r="B223" s="13"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="11"/>
+      <c r="F223" s="12"/>
+      <c r="G223" s="13"/>
+      <c r="H223" s="13"/>
+      <c r="I223" s="13"/>
+      <c r="J223" s="11"/>
+      <c r="K223" s="12"/>
+      <c r="L223" s="13"/>
+      <c r="M223" s="13"/>
+      <c r="N223" s="13"/>
+      <c r="O223" s="11"/>
+      <c r="P223" s="12"/>
+      <c r="Q223" s="13"/>
+      <c r="R223" s="13"/>
+      <c r="S223" s="13"/>
     </row>
     <row r="224" spans="1:19">
-      <c r="A224" s="5"/>
-      <c r="B224" s="6"/>
-      <c r="C224" s="6"/>
-      <c r="D224" s="6"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="5"/>
-      <c r="G224" s="6"/>
-      <c r="H224" s="6"/>
-      <c r="I224" s="6"/>
-      <c r="J224" s="2"/>
-      <c r="K224" s="5"/>
-      <c r="L224" s="6"/>
-      <c r="M224" s="6"/>
-      <c r="N224" s="6"/>
-      <c r="O224" s="2"/>
-      <c r="P224" s="5"/>
-      <c r="Q224" s="6"/>
-      <c r="R224" s="6"/>
-      <c r="S224" s="6"/>
+      <c r="A224" s="12"/>
+      <c r="B224" s="13"/>
+      <c r="C224" s="13"/>
+      <c r="D224" s="13"/>
+      <c r="E224" s="11"/>
+      <c r="F224" s="12"/>
+      <c r="G224" s="13"/>
+      <c r="H224" s="13"/>
+      <c r="I224" s="13"/>
+      <c r="J224" s="11"/>
+      <c r="K224" s="12"/>
+      <c r="L224" s="13"/>
+      <c r="M224" s="13"/>
+      <c r="N224" s="13"/>
+      <c r="O224" s="11"/>
+      <c r="P224" s="12"/>
+      <c r="Q224" s="13"/>
+      <c r="R224" s="13"/>
+      <c r="S224" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>